<commit_message>
Überarbeitung für Kurstag 5
</commit_message>
<xml_diff>
--- a/kurstag-05/Chemie_Messungen.xlsx
+++ b/kurstag-05/Chemie_Messungen.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frankzimmer/private/vhs-einfuehrung-julia-2023/kurstag-05/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D683EDD5-C1CB-3A42-BD8C-1549D1156DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="760" windowWidth="26980" windowHeight="16880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Messungen" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -40,8 +46,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,13 +110,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -148,7 +162,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -182,6 +196,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -216,9 +231,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -391,14 +407,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="C128" sqref="C128"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -412,7 +433,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -420,18 +441,18 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>100.9934283060225</v>
+        <v>100.99342830602249</v>
       </c>
       <c r="D2">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>2.040816326530612</v>
+        <v>2.0408163265306118</v>
       </c>
       <c r="C3">
         <v>95.72401552620542</v>
@@ -440,68 +461,68 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>4.081632653061225</v>
+        <v>4.0816326530612246</v>
       </c>
       <c r="C4">
-        <v>93.45642180597387</v>
+        <v>93.456421805973875</v>
       </c>
       <c r="D4">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>6.122448979591837</v>
+        <v>6.1224489795918373</v>
       </c>
       <c r="C5">
-        <v>91.52116412795193</v>
+        <v>91.521164127951934</v>
       </c>
       <c r="D5">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>8.163265306122449</v>
+        <v>8.1632653061224492</v>
       </c>
       <c r="C6">
-        <v>84.46827490738457</v>
+        <v>84.468274907384568</v>
       </c>
       <c r="D6">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7">
-        <v>10.20408163265306</v>
+        <v>10.204081632653059</v>
       </c>
       <c r="C7">
-        <v>81.07130664084794</v>
+        <v>81.071306640847936</v>
       </c>
       <c r="D7">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8">
-        <v>12.24489795918367</v>
+        <v>12.244897959183669</v>
       </c>
       <c r="C8">
         <v>81.43686664370675</v>
@@ -510,7 +531,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -518,102 +539,99 @@
         <v>14.28571428571429</v>
       </c>
       <c r="C9">
-        <v>76.68259876583441</v>
+        <v>76.682598765834413</v>
       </c>
       <c r="D9">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10">
-        <v>16.3265306122449</v>
-      </c>
-      <c r="C10">
-        <v>71.20328026360572</v>
+        <v>16.326530612244898</v>
       </c>
       <c r="D10">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11">
-        <v>18.36734693877551</v>
+        <v>18.367346938775508</v>
       </c>
       <c r="C11">
-        <v>70.3420525076917</v>
+        <v>70.342052507691704</v>
       </c>
       <c r="D11">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
       <c r="B12">
-        <v>20.40816326530612</v>
+        <v>20.408163265306118</v>
       </c>
       <c r="C12">
-        <v>65.56019658481466</v>
+        <v>65.560196584814662</v>
       </c>
       <c r="D12">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13">
-        <v>22.44897959183674</v>
+        <v>22.448979591836739</v>
       </c>
       <c r="C13">
-        <v>62.89645295940301</v>
+        <v>62.896452959403007</v>
       </c>
       <c r="D13">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
       <c r="B14">
-        <v>24.48979591836735</v>
+        <v>24.489795918367349</v>
       </c>
       <c r="C14">
-        <v>61.75906781690703</v>
+        <v>61.759067816907027</v>
       </c>
       <c r="D14">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
       <c r="B15">
-        <v>26.53061224489796</v>
+        <v>26.530612244897959</v>
       </c>
       <c r="C15">
-        <v>54.9979104690556</v>
+        <v>54.997910469055597</v>
       </c>
       <c r="D15">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
       <c r="B16">
-        <v>28.57142857142857</v>
+        <v>28.571428571428569</v>
       </c>
       <c r="C16">
         <v>53.02197653574985</v>
@@ -622,54 +640,51 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17">
-        <v>30.61224489795918</v>
+        <v>30.612244897959179</v>
       </c>
       <c r="C17">
-        <v>53.08867193351457</v>
+        <v>53.088671933514568</v>
       </c>
       <c r="D17">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
       <c r="B18">
-        <v>32.6530612244898</v>
+        <v>32.653061224489797</v>
       </c>
       <c r="C18">
-        <v>50.01934986140136</v>
+        <v>50.019349861401359</v>
       </c>
       <c r="D18">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
       <c r="B19">
-        <v>34.69387755102041</v>
-      </c>
-      <c r="C19">
-        <v>50.59198947494649</v>
+        <v>34.693877551020407</v>
       </c>
       <c r="D19">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
       <c r="B20">
-        <v>36.73469387755102</v>
+        <v>36.734693877551017</v>
       </c>
       <c r="C20">
         <v>46.14917873196201</v>
@@ -678,26 +693,26 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
       <c r="B21">
-        <v>38.77551020408163</v>
+        <v>38.775510204081627</v>
       </c>
       <c r="C21">
-        <v>43.22227139750614</v>
+        <v>43.222271397506141</v>
       </c>
       <c r="D21">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
       <c r="B22">
-        <v>40.81632653061224</v>
+        <v>40.816326530612237</v>
       </c>
       <c r="C22">
         <v>47.13655174022567</v>
@@ -706,26 +721,26 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
       <c r="B23">
-        <v>42.85714285714286</v>
+        <v>42.857142857142861</v>
       </c>
       <c r="C23">
-        <v>41.98573196672191</v>
+        <v>41.985731966721907</v>
       </c>
       <c r="D23">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
       <c r="B24">
-        <v>44.89795918367347</v>
+        <v>44.897959183673471</v>
       </c>
       <c r="C24">
         <v>40.87508050774327</v>
@@ -734,82 +749,82 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
       <c r="B25">
-        <v>46.93877551020408</v>
+        <v>46.938775510204081</v>
       </c>
       <c r="C25">
-        <v>36.26114844010731</v>
+        <v>36.261148440107313</v>
       </c>
       <c r="D25">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
       <c r="B26">
-        <v>48.9795918367347</v>
+        <v>48.979591836734699</v>
       </c>
       <c r="C26">
-        <v>36.45766638316613</v>
+        <v>36.457666383166128</v>
       </c>
       <c r="D26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
       <c r="B27">
-        <v>51.02040816326531</v>
+        <v>51.020408163265309</v>
       </c>
       <c r="C27">
-        <v>36.26662403920184</v>
+        <v>36.266624039201837</v>
       </c>
       <c r="D27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
       <c r="B28">
-        <v>53.06122448979592</v>
+        <v>53.061224489795919</v>
       </c>
       <c r="C28">
-        <v>32.30119668047797</v>
+        <v>32.301196680477972</v>
       </c>
       <c r="D28">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
       <c r="B29">
-        <v>55.10204081632653</v>
+        <v>55.102040816326529</v>
       </c>
       <c r="C29">
-        <v>33.97064080440271</v>
+        <v>33.970640804402713</v>
       </c>
       <c r="D29">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
       <c r="B30">
-        <v>57.14285714285715</v>
+        <v>57.142857142857153</v>
       </c>
       <c r="C30">
         <v>30.68937835255943</v>
@@ -818,40 +833,40 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>4</v>
       </c>
       <c r="B31">
-        <v>59.18367346938776</v>
+        <v>59.183673469387763</v>
       </c>
       <c r="C31">
-        <v>30.03181552967652</v>
+        <v>30.031815529676521</v>
       </c>
       <c r="D31">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
       <c r="B32">
-        <v>61.22448979591837</v>
+        <v>61.224489795918373</v>
       </c>
       <c r="C32">
-        <v>28.18734826969339</v>
+        <v>28.187348269693391</v>
       </c>
       <c r="D32">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
       <c r="B33">
-        <v>63.26530612244898</v>
+        <v>63.265306122448983</v>
       </c>
       <c r="C33">
         <v>31.91984732692768</v>
@@ -860,21 +875,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>4</v>
       </c>
       <c r="B34">
-        <v>65.30612244897959</v>
+        <v>65.306122448979593</v>
       </c>
       <c r="C34">
-        <v>27.05983839757048</v>
+        <v>27.059838397570481</v>
       </c>
       <c r="D34">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -888,96 +903,93 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>4</v>
       </c>
       <c r="B36">
-        <v>69.38775510204081</v>
+        <v>69.387755102040813</v>
       </c>
       <c r="C36">
-        <v>26.60859796025147</v>
+        <v>26.608597960251469</v>
       </c>
       <c r="D36">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>4</v>
       </c>
       <c r="B37">
-        <v>71.42857142857143</v>
+        <v>71.428571428571431</v>
       </c>
       <c r="C37">
-        <v>21.52341634423554</v>
+        <v>21.523416344235539</v>
       </c>
       <c r="D37">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>4</v>
       </c>
       <c r="B38">
-        <v>73.46938775510205</v>
+        <v>73.469387755102048</v>
       </c>
       <c r="C38">
-        <v>23.42435708939042</v>
+        <v>23.424357089390419</v>
       </c>
       <c r="D38">
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>4</v>
       </c>
       <c r="B39">
-        <v>75.51020408163265</v>
-      </c>
-      <c r="C39">
-        <v>18.16714964128729</v>
+        <v>75.510204081632651</v>
       </c>
       <c r="D39">
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>4</v>
       </c>
       <c r="B40">
-        <v>77.55102040816327</v>
+        <v>77.551020408163268</v>
       </c>
       <c r="C40">
-        <v>18.54677837458478</v>
+        <v>18.546778374584779</v>
       </c>
       <c r="D40">
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>4</v>
       </c>
       <c r="B41">
-        <v>79.59183673469389</v>
+        <v>79.591836734693885</v>
       </c>
       <c r="C41">
-        <v>20.74886229761937</v>
+        <v>20.748862297619372</v>
       </c>
       <c r="D41">
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>4</v>
       </c>
       <c r="B42">
-        <v>81.63265306122449</v>
+        <v>81.632653061224488</v>
       </c>
       <c r="C42">
         <v>21.01797815096344</v>
@@ -986,54 +998,54 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>4</v>
       </c>
       <c r="B43">
-        <v>83.67346938775511</v>
+        <v>83.673469387755105</v>
       </c>
       <c r="C43">
-        <v>19.10224608211798</v>
+        <v>19.102246082117979</v>
       </c>
       <c r="D43">
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>4</v>
       </c>
       <c r="B44">
-        <v>85.71428571428572</v>
+        <v>85.714285714285722</v>
       </c>
       <c r="C44">
-        <v>17.77793465001876</v>
+        <v>17.777934650018761</v>
       </c>
       <c r="D44">
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>4</v>
       </c>
       <c r="B45">
-        <v>87.75510204081633</v>
+        <v>87.755102040816325</v>
       </c>
       <c r="C45">
-        <v>16.68675256839312</v>
+        <v>16.686752568393121</v>
       </c>
       <c r="D45">
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>4</v>
       </c>
       <c r="B46">
-        <v>89.79591836734694</v>
+        <v>89.795918367346943</v>
       </c>
       <c r="C46">
         <v>13.64045165462073</v>
@@ -1042,7 +1054,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -1056,21 +1068,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>4</v>
       </c>
       <c r="B48">
-        <v>93.87755102040816</v>
+        <v>93.877551020408163</v>
       </c>
       <c r="C48">
-        <v>14.37514783460252</v>
+        <v>14.375147834602521</v>
       </c>
       <c r="D48">
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -1078,18 +1090,18 @@
         <v>95.91836734693878</v>
       </c>
       <c r="C49">
-        <v>16.7988960461163</v>
+        <v>16.798896046116301</v>
       </c>
       <c r="D49">
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>4</v>
       </c>
       <c r="B50">
-        <v>97.9591836734694</v>
+        <v>97.959183673469397</v>
       </c>
       <c r="C50">
         <v>14.78458201244972</v>
@@ -1098,7 +1110,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -1112,7 +1124,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -1120,97 +1132,97 @@
         <v>0</v>
       </c>
       <c r="C52">
-        <v>50.48612595409219</v>
+        <v>50.486125954092188</v>
       </c>
       <c r="D52">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>5</v>
       </c>
       <c r="B53">
-        <v>2.040816326530612</v>
+        <v>2.0408163265306118</v>
       </c>
       <c r="C53">
-        <v>47.91495483274981</v>
+        <v>47.914954832749807</v>
       </c>
       <c r="D53">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>5</v>
       </c>
       <c r="B54">
-        <v>4.081632653061225</v>
+        <v>4.0816326530612246</v>
       </c>
       <c r="C54">
-        <v>46.01521991273363</v>
+        <v>46.015219912733627</v>
       </c>
       <c r="D54">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>5</v>
       </c>
       <c r="B55">
-        <v>6.122448979591837</v>
+        <v>6.1224489795918373</v>
       </c>
       <c r="C55">
-        <v>46.53021827468856</v>
+        <v>46.530218274688558</v>
       </c>
       <c r="D55">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>5</v>
       </c>
       <c r="B56">
-        <v>8.163265306122449</v>
+        <v>8.1632653061224492</v>
       </c>
       <c r="C56">
-        <v>45.78405149131187</v>
+        <v>45.784051491311871</v>
       </c>
       <c r="D56">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>5</v>
       </c>
       <c r="B57">
-        <v>10.20408163265306</v>
+        <v>10.204081632653059</v>
       </c>
       <c r="C57">
-        <v>44.30077942193867</v>
+        <v>44.300779421938671</v>
       </c>
       <c r="D57">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>5</v>
       </c>
       <c r="B58">
-        <v>12.24489795918367</v>
+        <v>12.244897959183669</v>
       </c>
       <c r="C58">
-        <v>40.35154874968111</v>
+        <v>40.351548749681108</v>
       </c>
       <c r="D58">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -1218,363 +1230,357 @@
         <v>14.28571428571429</v>
       </c>
       <c r="C59">
-        <v>39.89206878649264</v>
+        <v>39.892068786492644</v>
       </c>
       <c r="D59">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>5</v>
       </c>
       <c r="B60">
-        <v>16.3265306122449</v>
+        <v>16.326530612244898</v>
       </c>
       <c r="C60">
-        <v>39.63611565345133</v>
+        <v>39.636115653451327</v>
       </c>
       <c r="D60">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>5</v>
       </c>
       <c r="B61">
-        <v>18.36734693877551</v>
+        <v>18.367346938775508</v>
       </c>
       <c r="C61">
-        <v>39.42255195428462</v>
+        <v>39.422551954284621</v>
       </c>
       <c r="D61">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>5</v>
       </c>
       <c r="B62">
-        <v>20.40816326530612</v>
+        <v>20.408163265306118</v>
       </c>
       <c r="C62">
-        <v>36.09606140254891</v>
+        <v>36.096061402548912</v>
       </c>
       <c r="D62">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>5</v>
       </c>
       <c r="B63">
-        <v>22.44897959183674</v>
+        <v>22.448979591836739</v>
       </c>
       <c r="C63">
-        <v>35.4264250058098</v>
+        <v>35.426425005809797</v>
       </c>
       <c r="D63">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>5</v>
       </c>
       <c r="B64">
-        <v>24.48979591836735</v>
+        <v>24.489795918367349</v>
       </c>
       <c r="C64">
-        <v>32.96896374925085</v>
+        <v>32.968963749250847</v>
       </c>
       <c r="D64">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>5</v>
       </c>
       <c r="B65">
-        <v>26.53061224489796</v>
-      </c>
-      <c r="C65">
-        <v>31.79016221378609</v>
+        <v>26.530612244897959</v>
       </c>
       <c r="D65">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>5</v>
       </c>
       <c r="B66">
-        <v>28.57142857142857</v>
+        <v>28.571428571428569</v>
       </c>
       <c r="C66">
-        <v>33.79074161014407</v>
+        <v>33.790741610144067</v>
       </c>
       <c r="D66">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>5</v>
       </c>
       <c r="B67">
-        <v>30.61224489795918</v>
+        <v>30.612244897959179</v>
       </c>
       <c r="C67">
         <v>33.62431951748534</v>
       </c>
       <c r="D67">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>5</v>
       </c>
       <c r="B68">
-        <v>32.6530612244898</v>
+        <v>32.653061224489797</v>
       </c>
       <c r="C68">
-        <v>30.52955645451698</v>
+        <v>30.529556454516982</v>
       </c>
       <c r="D68">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>5</v>
       </c>
       <c r="B69">
-        <v>34.69387755102041</v>
+        <v>34.693877551020407</v>
       </c>
       <c r="C69">
-        <v>31.21919614874057</v>
+        <v>31.219196148740568</v>
       </c>
       <c r="D69">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>5</v>
       </c>
       <c r="B70">
-        <v>36.73469387755102</v>
+        <v>36.734693877551017</v>
       </c>
       <c r="C70">
-        <v>29.36052335515038</v>
+        <v>29.360523355150381</v>
       </c>
       <c r="D70">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>5</v>
       </c>
       <c r="B71">
-        <v>38.77551020408163</v>
+        <v>38.775510204081627</v>
       </c>
       <c r="C71">
         <v>26.98156999796953</v>
       </c>
       <c r="D71">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>5</v>
       </c>
       <c r="B72">
-        <v>40.81632653061224</v>
+        <v>40.816326530612237</v>
       </c>
       <c r="C72">
         <v>27.64871690426088</v>
       </c>
       <c r="D72">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>5</v>
       </c>
       <c r="B73">
-        <v>42.85714285714286</v>
+        <v>42.857142857142861</v>
       </c>
       <c r="C73">
-        <v>28.59645607098794</v>
+        <v>28.596456070987941</v>
       </c>
       <c r="D73">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>5</v>
       </c>
       <c r="B74">
-        <v>44.89795918367347</v>
+        <v>44.897959183673471</v>
       </c>
       <c r="C74">
-        <v>25.44307786048927</v>
+        <v>25.443077860489272</v>
       </c>
       <c r="D74">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>5</v>
       </c>
       <c r="B75">
-        <v>46.93877551020408</v>
+        <v>46.938775510204081</v>
       </c>
       <c r="C75">
-        <v>27.07509327700186</v>
+        <v>27.075093277001859</v>
       </c>
       <c r="D75">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>5</v>
       </c>
       <c r="B76">
-        <v>48.9795918367347</v>
+        <v>48.979591836734699</v>
       </c>
       <c r="C76">
         <v>20.0529957853676</v>
       </c>
       <c r="D76">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>5</v>
       </c>
       <c r="B77">
-        <v>51.02040816326531</v>
+        <v>51.020408163265309</v>
       </c>
       <c r="C77">
-        <v>24.49242893721228</v>
+        <v>24.492428937212281</v>
       </c>
       <c r="D77">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>5</v>
       </c>
       <c r="B78">
-        <v>53.06122448979592</v>
-      </c>
-      <c r="C78">
-        <v>22.68890599411496</v>
+        <v>53.061224489795919</v>
       </c>
       <c r="D78">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>5</v>
       </c>
       <c r="B79">
-        <v>55.10204081632653</v>
+        <v>55.102040816326529</v>
       </c>
       <c r="C79">
-        <v>21.42972585931467</v>
+        <v>21.429725859314669</v>
       </c>
       <c r="D79">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>5</v>
       </c>
       <c r="B80">
-        <v>57.14285714285715</v>
+        <v>57.142857142857153</v>
       </c>
       <c r="C80">
         <v>21.35628344865075</v>
       </c>
       <c r="D80">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>5</v>
       </c>
       <c r="B81">
-        <v>59.18367346938776</v>
+        <v>59.183673469387763</v>
       </c>
       <c r="C81">
-        <v>17.59758005569529</v>
+        <v>17.597580055695289</v>
       </c>
       <c r="D81">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>5</v>
       </c>
       <c r="B82">
-        <v>61.22448979591837</v>
+        <v>61.224489795918373</v>
       </c>
       <c r="C82">
-        <v>19.62900296041792</v>
+        <v>19.629002960417921</v>
       </c>
       <c r="D82">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>5</v>
       </c>
       <c r="B83">
-        <v>63.26530612244898</v>
+        <v>63.265306122448983</v>
       </c>
       <c r="C83">
-        <v>19.89246178547405</v>
+        <v>19.892461785474051</v>
       </c>
       <c r="D83">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>5</v>
       </c>
       <c r="B84">
-        <v>65.30612244897959</v>
+        <v>65.306122448979593</v>
       </c>
       <c r="C84">
-        <v>20.99005698322052</v>
+        <v>20.990056983220519</v>
       </c>
       <c r="D84">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>5</v>
       </c>
@@ -1582,167 +1588,167 @@
         <v>67.34693877551021</v>
       </c>
       <c r="C85">
-        <v>17.42982751017695</v>
+        <v>17.429827510176949</v>
       </c>
       <c r="D85">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>5</v>
       </c>
       <c r="B86">
-        <v>69.38775510204081</v>
+        <v>69.387755102040813</v>
       </c>
       <c r="C86">
-        <v>16.44557285874249</v>
+        <v>16.445572858742491</v>
       </c>
       <c r="D86">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>5</v>
       </c>
       <c r="B87">
-        <v>71.42857142857143</v>
+        <v>71.428571428571431</v>
       </c>
       <c r="C87">
-        <v>16.37330718927547</v>
+        <v>16.373307189275469</v>
       </c>
       <c r="D87">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>5</v>
       </c>
       <c r="B88">
-        <v>73.46938775510205</v>
+        <v>73.469387755102048</v>
       </c>
       <c r="C88">
-        <v>17.98272556040879</v>
+        <v>17.982725560408792</v>
       </c>
       <c r="D88">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>5</v>
       </c>
       <c r="B89">
-        <v>75.51020408163265</v>
+        <v>75.510204081632651</v>
       </c>
       <c r="C89">
-        <v>16.6019949286519</v>
+        <v>16.601994928651902</v>
       </c>
       <c r="D89">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>5</v>
       </c>
       <c r="B90">
-        <v>77.55102040816327</v>
+        <v>77.551020408163268</v>
       </c>
       <c r="C90">
         <v>14.82857079181327</v>
       </c>
       <c r="D90">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>5</v>
       </c>
       <c r="B91">
-        <v>79.59183673469389</v>
+        <v>79.591836734693885</v>
       </c>
       <c r="C91">
         <v>15.92209688392504</v>
       </c>
       <c r="D91">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>5</v>
       </c>
       <c r="B92">
-        <v>81.63265306122449</v>
+        <v>81.632653061224488</v>
       </c>
       <c r="C92">
-        <v>14.84099707109815</v>
+        <v>14.840997071098149</v>
       </c>
       <c r="D92">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>5</v>
       </c>
       <c r="B93">
-        <v>83.67346938775511</v>
+        <v>83.673469387755105</v>
       </c>
       <c r="C93">
         <v>15.70530550261368</v>
       </c>
       <c r="D93">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>5</v>
       </c>
       <c r="B94">
-        <v>85.71428571428572</v>
+        <v>85.714285714285722</v>
       </c>
       <c r="C94">
-        <v>12.76957269066219</v>
+        <v>12.769572690662191</v>
       </c>
       <c r="D94">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>5</v>
       </c>
       <c r="B95">
-        <v>87.75510204081633</v>
+        <v>87.755102040816325</v>
       </c>
       <c r="C95">
         <v>12.91442777717123</v>
       </c>
       <c r="D95">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>5</v>
       </c>
       <c r="B96">
-        <v>89.79591836734694</v>
+        <v>89.795918367346943</v>
       </c>
       <c r="C96">
         <v>12.41359123047912</v>
       </c>
       <c r="D96">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>5</v>
       </c>
@@ -1750,27 +1756,27 @@
         <v>91.83673469387756</v>
       </c>
       <c r="C97">
-        <v>10.41449851977642</v>
+        <v>10.414498519776419</v>
       </c>
       <c r="D97">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>5</v>
       </c>
       <c r="B98">
-        <v>93.87755102040816</v>
+        <v>93.877551020408163</v>
       </c>
       <c r="C98">
-        <v>12.67378649881343</v>
+        <v>12.673786498813429</v>
       </c>
       <c r="D98">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>5</v>
       </c>
@@ -1778,27 +1784,27 @@
         <v>95.91836734693878</v>
       </c>
       <c r="C99">
-        <v>12.25248550823627</v>
+        <v>12.252485508236269</v>
       </c>
       <c r="D99">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>5</v>
       </c>
       <c r="B100">
-        <v>97.9591836734694</v>
+        <v>97.959183673469397</v>
       </c>
       <c r="C100">
-        <v>11.51098513465415</v>
+        <v>11.510985134654151</v>
       </c>
       <c r="D100">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>5</v>
       </c>
@@ -1809,10 +1815,10 @@
         <v>10.80462730735877</v>
       </c>
       <c r="D101">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>6</v>
       </c>
@@ -1820,97 +1826,94 @@
         <v>0</v>
       </c>
       <c r="C102">
-        <v>76.46157314487397</v>
+        <v>76.461573144873967</v>
       </c>
       <c r="D102">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>6</v>
       </c>
       <c r="B103">
-        <v>2.040816326530612</v>
+        <v>2.0408163265306118</v>
       </c>
       <c r="C103">
-        <v>77.33228060138296</v>
+        <v>77.332280601382962</v>
       </c>
       <c r="D103">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>6</v>
       </c>
       <c r="B104">
-        <v>4.081632653061225</v>
+        <v>4.0816326530612246</v>
       </c>
       <c r="C104">
-        <v>75.9436490115213</v>
+        <v>75.943649011521302</v>
       </c>
       <c r="D104">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>6</v>
       </c>
       <c r="B105">
-        <v>6.122448979591837</v>
+        <v>6.1224489795918373</v>
       </c>
       <c r="C105">
-        <v>73.24327148805406</v>
+        <v>73.243271488054063</v>
       </c>
       <c r="D105">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>6</v>
       </c>
       <c r="B106">
-        <v>8.163265306122449</v>
+        <v>8.1632653061224492</v>
       </c>
       <c r="C106">
-        <v>73.32562150465296</v>
+        <v>73.325621504652958</v>
       </c>
       <c r="D106">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>6</v>
       </c>
       <c r="B107">
-        <v>10.20408163265306</v>
+        <v>10.204081632653059</v>
       </c>
       <c r="C107">
         <v>73.24954266779875</v>
       </c>
       <c r="D107">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>6</v>
       </c>
       <c r="B108">
-        <v>12.24489795918367</v>
-      </c>
-      <c r="C108">
-        <v>75.49554828513503</v>
+        <v>12.244897959183669</v>
       </c>
       <c r="D108">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>6</v>
       </c>
@@ -1918,363 +1921,360 @@
         <v>14.28571428571429</v>
       </c>
       <c r="C109">
-        <v>69.78667651209412</v>
+        <v>69.786676512094118</v>
       </c>
       <c r="D109">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>6</v>
       </c>
       <c r="B110">
-        <v>16.3265306122449</v>
+        <v>16.326530612244898</v>
       </c>
       <c r="C110">
-        <v>68.5931413022719</v>
+        <v>68.593141302271903</v>
       </c>
       <c r="D110">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>6</v>
       </c>
       <c r="B111">
-        <v>18.36734693877551</v>
+        <v>18.367346938775508</v>
       </c>
       <c r="C111">
-        <v>66.39048526580869</v>
+        <v>66.390485265808692</v>
       </c>
       <c r="D111">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>6</v>
       </c>
       <c r="B112">
-        <v>20.40816326530612</v>
+        <v>20.408163265306118</v>
       </c>
       <c r="C112">
         <v>60.43473640554943</v>
       </c>
       <c r="D112">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>6</v>
       </c>
       <c r="B113">
-        <v>22.44897959183674</v>
+        <v>22.448979591836739</v>
       </c>
       <c r="C113">
         <v>63.84761362667912</v>
       </c>
       <c r="D113">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>6</v>
       </c>
       <c r="B114">
-        <v>24.48979591836735</v>
+        <v>24.489795918367349</v>
       </c>
       <c r="C114">
-        <v>62.77332833500613</v>
+        <v>62.773328335006127</v>
       </c>
       <c r="D114">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>6</v>
       </c>
       <c r="B115">
-        <v>26.53061224489796</v>
+        <v>26.530612244897959</v>
       </c>
       <c r="C115">
-        <v>67.51579543767004</v>
+        <v>67.515795437670036</v>
       </c>
       <c r="D115">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>6</v>
       </c>
       <c r="B116">
-        <v>28.57142857142857</v>
+        <v>28.571428571428569</v>
       </c>
       <c r="C116">
-        <v>59.63728103407008</v>
+        <v>59.637281034070078</v>
       </c>
       <c r="D116">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>6</v>
       </c>
       <c r="B117">
-        <v>30.61224489795918</v>
+        <v>30.612244897959179</v>
       </c>
       <c r="C117">
-        <v>59.65758477074097</v>
+        <v>59.657584770740968</v>
       </c>
       <c r="D117">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>6</v>
       </c>
       <c r="B118">
-        <v>32.6530612244898</v>
+        <v>32.653061224489797</v>
       </c>
       <c r="C118">
-        <v>57.62700380411739</v>
+        <v>57.627003804117393</v>
       </c>
       <c r="D118">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>6</v>
       </c>
       <c r="B119">
-        <v>34.69387755102041</v>
+        <v>34.693877551020407</v>
       </c>
       <c r="C119">
-        <v>53.62619317619854</v>
+        <v>53.626193176198541</v>
       </c>
       <c r="D119">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>6</v>
       </c>
       <c r="B120">
-        <v>36.73469387755102</v>
+        <v>36.734693877551017</v>
       </c>
       <c r="C120">
-        <v>58.26260297270336</v>
+        <v>58.262602972703363</v>
       </c>
       <c r="D120">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>6</v>
       </c>
       <c r="B121">
-        <v>38.77551020408163</v>
+        <v>38.775510204081627</v>
       </c>
       <c r="C121">
-        <v>56.16611301435764</v>
+        <v>56.166113014357641</v>
       </c>
       <c r="D121">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>6</v>
       </c>
       <c r="B122">
-        <v>40.81632653061224</v>
+        <v>40.816326530612237</v>
       </c>
       <c r="C122">
         <v>55.16720544395929</v>
       </c>
       <c r="D122">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>6</v>
       </c>
       <c r="B123">
-        <v>42.85714285714286</v>
+        <v>42.857142857142861</v>
       </c>
       <c r="C123">
-        <v>49.84165596549759</v>
+        <v>49.841655965497587</v>
       </c>
       <c r="D123">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>6</v>
       </c>
       <c r="B124">
-        <v>44.89795918367347</v>
+        <v>44.897959183673471</v>
       </c>
       <c r="C124">
-        <v>54.56931575057506</v>
+        <v>54.569315750575058</v>
       </c>
       <c r="D124">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>6</v>
       </c>
       <c r="B125">
-        <v>46.93877551020408</v>
+        <v>46.938775510204081</v>
       </c>
       <c r="C125">
-        <v>46.52617553467503</v>
+        <v>46.526175534675033</v>
       </c>
       <c r="D125">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>6</v>
       </c>
       <c r="B126">
-        <v>48.9795918367347</v>
+        <v>48.979591836734699</v>
       </c>
       <c r="C126">
         <v>50.48725735352064</v>
       </c>
       <c r="D126">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>6</v>
       </c>
       <c r="B127">
-        <v>51.02040816326531</v>
+        <v>51.020408163265309</v>
       </c>
       <c r="C127">
-        <v>53.5059823603973</v>
+        <v>53.505982360397297</v>
       </c>
       <c r="D127">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>6</v>
       </c>
       <c r="B128">
-        <v>53.06122448979592</v>
-      </c>
-      <c r="C128">
-        <v>44.58323595387024</v>
+        <v>53.061224489795919</v>
       </c>
       <c r="D128">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>6</v>
       </c>
       <c r="B129">
-        <v>55.10204081632653</v>
+        <v>55.102040816326529</v>
       </c>
       <c r="C129">
-        <v>44.69316658411935</v>
+        <v>44.693166584119354</v>
       </c>
       <c r="D129">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>6</v>
       </c>
       <c r="B130">
-        <v>57.14285714285715</v>
+        <v>57.142857142857153</v>
       </c>
       <c r="C130">
-        <v>45.42657817333983</v>
+        <v>45.426578173339827</v>
       </c>
       <c r="D130">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>6</v>
       </c>
       <c r="B131">
-        <v>59.18367346938776</v>
+        <v>59.183673469387763</v>
       </c>
       <c r="C131">
-        <v>43.00611622825806</v>
+        <v>43.006116228258058</v>
       </c>
       <c r="D131">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>6</v>
       </c>
       <c r="B132">
-        <v>61.22448979591837</v>
+        <v>61.224489795918373</v>
       </c>
       <c r="C132">
-        <v>39.49393901593188</v>
+        <v>39.493939015931879</v>
       </c>
       <c r="D132">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>6</v>
       </c>
       <c r="B133">
-        <v>63.26530612244898</v>
+        <v>63.265306122448983</v>
       </c>
       <c r="C133">
-        <v>42.66586144346427</v>
+        <v>42.665861443464273</v>
       </c>
       <c r="D133">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>6</v>
       </c>
       <c r="B134">
-        <v>65.30612244897959</v>
+        <v>65.306122448979593</v>
       </c>
       <c r="C134">
         <v>38.98025039734091</v>
       </c>
       <c r="D134">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>6</v>
       </c>
@@ -2282,167 +2282,164 @@
         <v>67.34693877551021</v>
       </c>
       <c r="C135">
-        <v>41.97888814723466</v>
+        <v>41.978888147234663</v>
       </c>
       <c r="D135">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>6</v>
       </c>
       <c r="B136">
-        <v>69.38775510204081</v>
+        <v>69.387755102040813</v>
       </c>
       <c r="C136">
-        <v>37.67223526222025</v>
+        <v>37.672235262220248</v>
       </c>
       <c r="D136">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>6</v>
       </c>
       <c r="B137">
-        <v>71.42857142857143</v>
+        <v>71.428571428571431</v>
       </c>
       <c r="C137">
-        <v>43.0381687771001</v>
+        <v>43.038168777100097</v>
       </c>
       <c r="D137">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>6</v>
       </c>
       <c r="B138">
-        <v>73.46938775510205</v>
+        <v>73.469387755102048</v>
       </c>
       <c r="C138">
-        <v>36.41404827556295</v>
+        <v>36.414048275562948</v>
       </c>
       <c r="D138">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>6</v>
       </c>
       <c r="B139">
-        <v>75.51020408163265</v>
+        <v>75.510204081632651</v>
       </c>
       <c r="C139">
-        <v>36.79185876233364</v>
+        <v>36.791858762333639</v>
       </c>
       <c r="D139">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>6</v>
       </c>
       <c r="B140">
-        <v>77.55102040816327</v>
+        <v>77.551020408163268</v>
       </c>
       <c r="C140">
-        <v>38.87129608356555</v>
+        <v>38.871296083565547</v>
       </c>
       <c r="D140">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>6</v>
       </c>
       <c r="B141">
-        <v>79.59183673469389</v>
+        <v>79.591836734693885</v>
       </c>
       <c r="C141">
-        <v>33.01617583572744</v>
+        <v>33.016175835727438</v>
       </c>
       <c r="D141">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>6</v>
       </c>
       <c r="B142">
-        <v>81.63265306122449</v>
-      </c>
-      <c r="C142">
-        <v>35.93285319841637</v>
+        <v>81.632653061224488</v>
       </c>
       <c r="D142">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>6</v>
       </c>
       <c r="B143">
-        <v>83.67346938775511</v>
+        <v>83.673469387755105</v>
       </c>
       <c r="C143">
-        <v>37.91765644159433</v>
+        <v>37.917656441594332</v>
       </c>
       <c r="D143">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>6</v>
       </c>
       <c r="B144">
-        <v>85.71428571428572</v>
+        <v>85.714285714285722</v>
       </c>
       <c r="C144">
-        <v>29.93111956775292</v>
+        <v>29.931119567752919</v>
       </c>
       <c r="D144">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>6</v>
       </c>
       <c r="B145">
-        <v>87.75510204081633</v>
+        <v>87.755102040816325</v>
       </c>
       <c r="C145">
-        <v>33.72558075943463</v>
+        <v>33.725580759434628</v>
       </c>
       <c r="D145">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>6</v>
       </c>
       <c r="B146">
-        <v>89.79591836734694</v>
+        <v>89.795918367346943</v>
       </c>
       <c r="C146">
-        <v>33.241726264315</v>
+        <v>33.241726264314998</v>
       </c>
       <c r="D146">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>6</v>
       </c>
@@ -2450,27 +2447,27 @@
         <v>91.83673469387756</v>
       </c>
       <c r="C147">
-        <v>33.88817444692196</v>
+        <v>33.888174446921958</v>
       </c>
       <c r="D147">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>6</v>
       </c>
       <c r="B148">
-        <v>93.87755102040816</v>
+        <v>93.877551020408163</v>
       </c>
       <c r="C148">
-        <v>28.19613907283217</v>
+        <v>28.196139072832171</v>
       </c>
       <c r="D148">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>6</v>
       </c>
@@ -2478,27 +2475,27 @@
         <v>95.91836734693878</v>
       </c>
       <c r="C149">
-        <v>27.35530480399674</v>
+        <v>27.355304803996741</v>
       </c>
       <c r="D149">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>6</v>
       </c>
       <c r="B150">
-        <v>97.9591836734694</v>
+        <v>97.959183673469397</v>
       </c>
       <c r="C150">
-        <v>31.34199937981544</v>
+        <v>31.341999379815441</v>
       </c>
       <c r="D150">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>6</v>
       </c>
@@ -2506,10 +2503,10 @@
         <v>100</v>
       </c>
       <c r="C151">
-        <v>30.17281697679836</v>
+        <v>30.172816976798359</v>
       </c>
       <c r="D151">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>